<commit_message>
Addition of test data parameter
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/stg/ManageClaims/ManageClaims.xlsx
+++ b/testdata/FCfiles/stg/ManageClaims/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="266">
   <si>
     <t>shipmentType</t>
   </si>
@@ -809,6 +809,24 @@
   </si>
   <si>
     <t>DropOff91</t>
+  </si>
+  <si>
+    <t>58571703</t>
+  </si>
+  <si>
+    <t>02-12-2022</t>
+  </si>
+  <si>
+    <t>FCT942112781459521536</t>
+  </si>
+  <si>
+    <t>FCTEST1004280</t>
+  </si>
+  <si>
+    <t>PickUp7</t>
+  </si>
+  <si>
+    <t>DropOff936</t>
   </si>
 </sst>
 </file>
@@ -837,7 +855,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="542">
+  <fills count="562">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3544,8 +3562,108 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="540">
+  <borders count="560">
     <border>
       <left/>
       <right/>
@@ -5676,11 +5794,81 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="296">
+  <cellXfs count="306">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -5976,7 +6164,17 @@
     <xf applyBorder="true" applyFill="true" borderId="533" fillId="535" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="535" fillId="537" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="537" fillId="539" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="541" borderId="539" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="539" fillId="541" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="541" fillId="543" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="543" fillId="545" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="545" fillId="547" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="547" fillId="549" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="549" fillId="551" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="551" fillId="553" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="553" fillId="555" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="555" fillId="557" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="557" fillId="559" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="561" borderId="559" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -6437,8 +6635,8 @@
       <c r="B2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="294" t="s">
-        <v>258</v>
+      <c r="C2" s="304" t="s">
+        <v>264</v>
       </c>
       <c r="D2" t="s">
         <v>114</v>
@@ -6461,8 +6659,8 @@
       <c r="J2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="295" t="s">
-        <v>259</v>
+      <c r="K2" s="305" t="s">
+        <v>265</v>
       </c>
       <c r="L2" t="s">
         <v>117</v>
@@ -6607,8 +6805,8 @@
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="288" t="s">
-        <v>255</v>
+      <c r="B2" s="298" t="s">
+        <v>261</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -6659,22 +6857,22 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="287" t="s">
-        <v>254</v>
-      </c>
-      <c r="U2" s="289" t="s">
+      <c r="T2" s="297" t="s">
+        <v>260</v>
+      </c>
+      <c r="U2" s="299" t="s">
         <v>195</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="290" t="s">
-        <v>256</v>
-      </c>
-      <c r="X2" s="291" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y2" s="292" t="s">
+      <c r="W2" s="300" t="s">
+        <v>262</v>
+      </c>
+      <c r="X2" s="301" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y2" s="302" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6907,7 +7105,7 @@
       <c r="B2" s="193" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="293" t="s">
+      <c r="C2" s="303" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="1" t="s">

</xml_diff>

<commit_message>
Overage new invoice amount logic change
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/stg/ManageClaims/ManageClaims.xlsx
+++ b/testdata/FCfiles/stg/ManageClaims/ManageClaims.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\testdata\FCfiles\stg\ManageClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{D9D24F22-0E3D-4D9E-9C0C-7BBA24922048}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{12952F09-C7A3-4394-A5DB-E411EC643D83}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView tabRatio="669" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="2" tabRatio="669" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="CreateAccount" r:id="rId1" sheetId="5"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="176">
   <si>
     <t>shipmentType</t>
   </si>
@@ -334,9 +334,6 @@
     <t>1234567890</t>
   </si>
   <si>
-    <t>FC Test Carrier</t>
-  </si>
-  <si>
     <t>PaymentMethod</t>
   </si>
   <si>
@@ -454,37 +451,67 @@
     <t>FCTEST1004430</t>
   </si>
   <si>
-    <t>59069932</t>
-  </si>
-  <si>
     <t>05-13-2022</t>
   </si>
   <si>
-    <t>FCTEST1004434</t>
-  </si>
-  <si>
-    <t>PickUp960</t>
-  </si>
-  <si>
-    <t>DropOff357</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
     <t>Automation</t>
   </si>
   <si>
-    <t>59069938</t>
-  </si>
-  <si>
-    <t>FCTEST1004435</t>
-  </si>
-  <si>
-    <t>PickUp113</t>
-  </si>
-  <si>
-    <t>DropOff594</t>
+    <t>Pending Documentation</t>
+  </si>
+  <si>
+    <t>59069939</t>
+  </si>
+  <si>
+    <t>FCTEST1004436</t>
+  </si>
+  <si>
+    <t>PickUp680</t>
+  </si>
+  <si>
+    <t>DropOff831</t>
+  </si>
+  <si>
+    <t>FragilePAK</t>
+  </si>
+  <si>
+    <t>59070314</t>
+  </si>
+  <si>
+    <t>05-18-2022</t>
+  </si>
+  <si>
+    <t>$694.99</t>
+  </si>
+  <si>
+    <t>999U668166</t>
+  </si>
+  <si>
+    <t>FCPBID1034610</t>
+  </si>
+  <si>
+    <t>PickUp992</t>
+  </si>
+  <si>
+    <t>DropOff805</t>
+  </si>
+  <si>
+    <t>59070315</t>
+  </si>
+  <si>
+    <t>999U668186</t>
+  </si>
+  <si>
+    <t>FCPBID1034611</t>
+  </si>
+  <si>
+    <t>PickUp936</t>
+  </si>
+  <si>
+    <t>DropOff873</t>
   </si>
   <si>
     <t>Review</t>
@@ -496,19 +523,40 @@
     <t>Filed - Review</t>
   </si>
   <si>
-    <t>Pending Documentation</t>
-  </si>
-  <si>
-    <t>59069939</t>
-  </si>
-  <si>
-    <t>FCTEST1004436</t>
-  </si>
-  <si>
-    <t>PickUp680</t>
-  </si>
-  <si>
-    <t>DropOff831</t>
+    <t>59070320</t>
+  </si>
+  <si>
+    <t>$663.63</t>
+  </si>
+  <si>
+    <t>999U668418</t>
+  </si>
+  <si>
+    <t>FCPBID1034612</t>
+  </si>
+  <si>
+    <t>PickUp967</t>
+  </si>
+  <si>
+    <t>DropOff97</t>
+  </si>
+  <si>
+    <t>59070322</t>
+  </si>
+  <si>
+    <t>$661.53</t>
+  </si>
+  <si>
+    <t>999U668528</t>
+  </si>
+  <si>
+    <t>FCPBID1034613</t>
+  </si>
+  <si>
+    <t>PickUp229</t>
+  </si>
+  <si>
+    <t>DropOff169</t>
   </si>
 </sst>
 </file>
@@ -537,7 +585,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="108">
+  <fills count="152">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1074,8 +1122,228 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="106">
+  <borders count="150">
     <border>
       <left/>
       <right/>
@@ -1687,11 +1955,165 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="101">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1770,7 +2192,29 @@
     <xf applyBorder="true" applyFill="true" borderId="99" fillId="101" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="101" fillId="103" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="103" fillId="105" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="107" borderId="105" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="105" fillId="107" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="107" fillId="109" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="109" fillId="111" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="111" fillId="113" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="113" fillId="115" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="115" fillId="117" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="117" fillId="119" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="119" fillId="121" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="121" fillId="123" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="123" fillId="125" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="125" fillId="127" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="127" fillId="129" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="129" fillId="131" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="131" fillId="133" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="133" fillId="135" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="135" fillId="137" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="137" fillId="139" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="139" fillId="141" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="141" fillId="143" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="143" fillId="145" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="145" fillId="147" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="147" fillId="149" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="151" borderId="149" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2053,7 +2497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2104,10 +2548,10 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
         <v>95</v>
@@ -2170,111 +2614,111 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" t="s">
-        <v>106</v>
-      </c>
-      <c r="J1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P1" t="s">
         <v>108</v>
       </c>
-      <c r="M1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R1" t="s">
         <v>130</v>
-      </c>
-      <c r="P1" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>110</v>
-      </c>
-      <c r="R1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="71" t="s">
-        <v>158</v>
+        <v>117</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="s">
         <v>125</v>
-      </c>
-      <c r="F2" t="s">
-        <v>126</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" t="s">
         <v>112</v>
-      </c>
-      <c r="I2" t="s">
-        <v>113</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="K2" s="72" t="s">
-        <v>159</v>
+      <c r="K2" s="100" t="s">
+        <v>175</v>
       </c>
       <c r="L2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M2" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" t="s">
         <v>132</v>
-      </c>
-      <c r="N2" t="s">
-        <v>133</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="P2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q2" t="s">
         <v>115</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>116</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>100</v>
@@ -2290,7 +2734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
@@ -2311,11 +2755,11 @@
     <col min="16" max="16" style="1" width="9.140625" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
     <col min="18" max="19" style="1" width="9.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="7.98828125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="9.9453125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="9.95703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.28125" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="15.25390625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="15.25390625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="12.484375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="15.265625" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="9.76171875" collapsed="true"/>
     <col min="26" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
@@ -2401,8 +2845,8 @@
       <c r="A2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="65" t="s">
-        <v>142</v>
+      <c r="B2" s="93" t="s">
+        <v>150</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -2453,31 +2897,31 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="U2" s="66" t="s">
+      <c r="T2" s="92" t="s">
+        <v>170</v>
+      </c>
+      <c r="U2" s="94" t="s">
+        <v>171</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="W2" s="95" t="s">
+        <v>172</v>
+      </c>
+      <c r="X2" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y2" s="97" t="s">
         <v>136</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="W2" s="67" t="s">
-        <v>157</v>
-      </c>
-      <c r="X2" s="68" t="s">
-        <v>157</v>
-      </c>
-      <c r="Y2" s="69" t="s">
-        <v>137</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>135</v>
+      <c r="B3" s="74" t="s">
+        <v>150</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -2528,22 +2972,22 @@
       <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>139</v>
+      <c r="T3" s="73" t="s">
+        <v>164</v>
+      </c>
+      <c r="U3" s="75" t="s">
+        <v>165</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="W3" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="X3" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y3" s="27"/>
+        <v>148</v>
+      </c>
+      <c r="W3" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="X3" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y3" s="78"/>
     </row>
     <row customHeight="1" ht="15.75" r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2604,7 +3048,7 @@
       </c>
       <c r="U4" s="9"/>
       <c r="V4" s="10" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="W4" s="19"/>
       <c r="X4" s="10"/>
@@ -2628,7 +3072,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.4296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5859375" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
@@ -2695,14 +3139,14 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="78" t="s">
-        <v>155</v>
+      <c r="B2" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="98" t="s">
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>43</v>
@@ -2739,14 +3183,14 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>134</v>
+      <c r="A3" s="82" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="88" t="s">
+        <v>133</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>78</v>
@@ -2865,7 +3309,7 @@
         <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2885,7 +3329,7 @@
         <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Addition of enable carrier script under BOL and logoff issue fix
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/stg/ManageClaims/ManageClaims.xlsx
+++ b/testdata/FCfiles/stg/ManageClaims/ManageClaims.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="216">
   <si>
     <t>shipmentType</t>
   </si>
@@ -656,6 +656,27 @@
   </si>
   <si>
     <t>DropOff3875</t>
+  </si>
+  <si>
+    <t>59075574</t>
+  </si>
+  <si>
+    <t>06-17-2022</t>
+  </si>
+  <si>
+    <t>$663.78</t>
+  </si>
+  <si>
+    <t>999U748301</t>
+  </si>
+  <si>
+    <t>FCPBID1034676</t>
+  </si>
+  <si>
+    <t>PickUp8399</t>
+  </si>
+  <si>
+    <t>DropOff7493</t>
   </si>
 </sst>
 </file>
@@ -684,7 +705,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="330">
+  <fills count="350">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2331,8 +2352,108 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="328">
+  <borders count="348">
     <border>
       <left/>
       <right/>
@@ -3721,11 +3842,81 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="200">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -3915,7 +4106,17 @@
     <xf applyBorder="true" applyFill="true" borderId="321" fillId="323" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="323" fillId="325" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="325" fillId="327" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="329" borderId="327" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="327" fillId="329" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="329" fillId="331" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="331" fillId="333" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="333" fillId="335" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="335" fillId="337" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="337" fillId="339" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="339" fillId="341" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="341" fillId="343" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="343" fillId="345" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="345" fillId="347" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="349" borderId="347" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -4376,8 +4577,8 @@
       <c r="B2" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="188" t="s">
-        <v>207</v>
+      <c r="C2" s="198" t="s">
+        <v>214</v>
       </c>
       <c r="D2" t="s">
         <v>110</v>
@@ -4400,8 +4601,8 @@
       <c r="J2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="K2" s="189" t="s">
-        <v>208</v>
+      <c r="K2" s="199" t="s">
+        <v>215</v>
       </c>
       <c r="L2" t="s">
         <v>113</v>
@@ -4546,8 +4747,8 @@
       <c r="A2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="182" t="s">
-        <v>189</v>
+      <c r="B2" s="192" t="s">
+        <v>210</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
@@ -4598,22 +4799,22 @@
       <c r="S2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="181" t="s">
-        <v>204</v>
-      </c>
-      <c r="U2" s="183" t="s">
-        <v>171</v>
+      <c r="T2" s="191" t="s">
+        <v>209</v>
+      </c>
+      <c r="U2" s="193" t="s">
+        <v>211</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="W2" s="184" t="s">
-        <v>205</v>
-      </c>
-      <c r="X2" s="185" t="s">
-        <v>206</v>
-      </c>
-      <c r="Y2" s="186" t="s">
+      <c r="W2" s="194" t="s">
+        <v>212</v>
+      </c>
+      <c r="X2" s="195" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y2" s="196" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4846,7 +5047,7 @@
       <c r="B2" s="155" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="197" t="s">
         <v>79</v>
       </c>
       <c r="D2" s="1" t="s">

</xml_diff>